<commit_message>
Added provider courses for 2021
</commit_message>
<xml_diff>
--- a/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
+++ b/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SFA\tl-marketing-and-communication\sfa.Tl.Marketing.Communication.DataLoad\Provider Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCC0B89-76B9-4749-B4A1-F16A51BC6DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E18084-B2FF-42C9-9C0C-2464098DA05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2205,8 +2205,8 @@
   <dimension ref="A1:P608"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A412" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G422" sqref="A422:XFD424"/>
+      <pane ySplit="1" topLeftCell="A589" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L608" sqref="L608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2592,7 +2592,7 @@
         <v>19</v>
       </c>
       <c r="O8" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>25</v>
@@ -10906,7 +10906,7 @@
         <v>19</v>
       </c>
       <c r="O182" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P182" s="3" t="s">
         <v>184</v>
@@ -24485,7 +24485,7 @@
         <v>19</v>
       </c>
       <c r="O469" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P469" s="3" t="s">
         <v>440</v>
@@ -24532,7 +24532,7 @@
         <v>19</v>
       </c>
       <c r="O470" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P470" s="3" t="s">
         <v>440</v>
@@ -28663,7 +28663,7 @@
         <v>19</v>
       </c>
       <c r="O557" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P557" s="3" t="s">
         <v>537</v>
@@ -30931,7 +30931,7 @@
         <v>19</v>
       </c>
       <c r="O605" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P605" s="3" t="s">
         <v>597</v>
@@ -31025,7 +31025,7 @@
         <v>19</v>
       </c>
       <c r="O607" s="2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="P607" s="3" t="s">
         <v>597</v>

</xml_diff>

<commit_message>
Update website for UCB
</commit_message>
<xml_diff>
--- a/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
+++ b/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esfa\tl-marketing-and-communication\sfa.Tl.Marketing.Communication.DataLoad\Provider Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F498F123-111E-4628-9849-07863CE66D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3BD05E-4008-40A2-AEF2-515455E3898B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32400" yWindow="1830" windowWidth="28515" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31725" yWindow="2505" windowWidth="19350" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Provider Data 2020 - 2021" sheetId="1" r:id="rId1"/>
@@ -1630,9 +1630,6 @@
     <t>B3 1JP</t>
   </si>
   <si>
-    <t>https://www.ucb.ac.uk/our-courses/college-courses/t-levels.aspx</t>
-  </si>
-  <si>
     <t>Ursuline High School</t>
   </si>
   <si>
@@ -1820,6 +1817,9 @@
   </si>
   <si>
     <t>https://www.osfc.ac.uk/courses/digital-t-level/</t>
+  </si>
+  <si>
+    <t>https://www.ucb.ac.uk/study/college/introducing-new-t-levels/</t>
   </si>
 </sst>
 </file>
@@ -2205,9 +2205,9 @@
   </sheetPr>
   <dimension ref="A1:P608"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O573" sqref="O573"/>
+      <selection pane="bottomLeft" activeCell="G557" sqref="A557:XFD557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2240,7 +2240,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -21246,7 +21246,7 @@
         <v>2020</v>
       </c>
       <c r="P400" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="401" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -21293,7 +21293,7 @@
         <v>2021</v>
       </c>
       <c r="P401" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="402" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22280,7 +22280,7 @@
         <v>2021</v>
       </c>
       <c r="P422" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="423" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22327,7 +22327,7 @@
         <v>2021</v>
       </c>
       <c r="P423" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="424" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22374,7 +22374,7 @@
         <v>2020</v>
       </c>
       <c r="P424" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="425" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28666,8 +28666,8 @@
       <c r="O557" s="2">
         <v>2021</v>
       </c>
-      <c r="P557" s="3" t="s">
-        <v>536</v>
+      <c r="P557" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="558" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28713,19 +28713,19 @@
       <c r="O558" s="2">
         <v>2021</v>
       </c>
-      <c r="P558" s="3" t="s">
-        <v>536</v>
+      <c r="P558" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="559" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A559" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C559" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="C559" s="2" t="s">
+      <c r="D559" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="D559" s="2" t="s">
-        <v>539</v>
       </c>
       <c r="E559" s="2" t="s">
         <v>18</v>
@@ -28761,159 +28761,159 @@
         <v>2020</v>
       </c>
       <c r="P559" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="560" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A560" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C560" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="C560" s="2" t="s">
+      <c r="D560" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D560" s="2" t="s">
+      <c r="E560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G560" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N560" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O560" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P560" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="E560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G560" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N560" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O560" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P560" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="561" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A561" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C561" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="C561" s="2" t="s">
+      <c r="D561" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D561" s="2" t="s">
+      <c r="E561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H561" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N561" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O561" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P561" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="E561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H561" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N561" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O561" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P561" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="562" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A562" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C562" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="C562" s="2" t="s">
+      <c r="D562" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D562" s="2" t="s">
+      <c r="E562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K562" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N562" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O562" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P562" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="E562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K562" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N562" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O562" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P562" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="563" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A563" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C563" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C563" s="2" t="s">
+      <c r="D563" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="D563" s="2" t="s">
-        <v>547</v>
       </c>
       <c r="E563" s="2" t="s">
         <v>18</v>
@@ -28949,112 +28949,112 @@
         <v>2020</v>
       </c>
       <c r="P563" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="564" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A564" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C564" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C564" s="2" t="s">
+      <c r="D564" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D564" s="2" t="s">
+      <c r="E564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G564" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O564" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P564" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G564" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O564" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P564" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="565" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A565" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C565" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C565" s="2" t="s">
+      <c r="D565" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D565" s="2" t="s">
+      <c r="E565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F565" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O565" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P565" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F565" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O565" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P565" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="566" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A566" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C566" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C566" s="2" t="s">
+      <c r="D566" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="D566" s="2" t="s">
-        <v>547</v>
       </c>
       <c r="E566" s="2" t="s">
         <v>19</v>
@@ -29090,159 +29090,159 @@
         <v>2020</v>
       </c>
       <c r="P566" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="567" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A567" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C567" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C567" s="2" t="s">
+      <c r="D567" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D567" s="2" t="s">
+      <c r="E567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L567" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O567" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P567" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L567" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O567" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P567" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="568" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A568" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C568" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C568" s="2" t="s">
+      <c r="D568" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D568" s="2" t="s">
+      <c r="E568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M568" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O568" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P568" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M568" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O568" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P568" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="569" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A569" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C569" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="C569" s="2" t="s">
+      <c r="D569" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D569" s="2" t="s">
+      <c r="E569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N569" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O569" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P569" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N569" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O569" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P569" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="570" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A570" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C570" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D570" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E570" s="2" t="s">
         <v>19</v>
@@ -29278,213 +29278,213 @@
         <v>2020</v>
       </c>
       <c r="P570" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="571" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A571" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C571" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D571" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I571" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O571" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P571" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="E571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I571" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O571" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P571" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="572" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A572" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C572" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="C572" s="2" t="s">
+      <c r="D572" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F572" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O572" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P572" s="3" t="s">
         <v>551</v>
-      </c>
-      <c r="D572" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F572" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O572" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P572" s="3" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="573" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A573" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C573" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="C573" s="2" t="s">
+      <c r="D573" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E573" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O573" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P573" s="3" t="s">
         <v>551</v>
-      </c>
-      <c r="D573" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="E573" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O573" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P573" s="3" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="574" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A574" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B574" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="B574" s="2" t="s">
+      <c r="C574" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="C574" s="2" t="s">
+      <c r="D574" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="D574" s="2" t="s">
+      <c r="E574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G574" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O574" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P574" s="3" t="s">
         <v>556</v>
-      </c>
-      <c r="E574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G574" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O574" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P574" s="3" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="575" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A575" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B575" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C575" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C575" s="2" t="s">
+      <c r="D575" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D575" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="E575" s="2" t="s">
         <v>19</v>
       </c>
@@ -29519,22 +29519,22 @@
         <v>2021</v>
       </c>
       <c r="P575" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="576" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A576" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B576" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C576" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C576" s="2" t="s">
+      <c r="D576" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D576" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="E576" s="2" t="s">
         <v>18</v>
       </c>
@@ -29569,22 +29569,22 @@
         <v>2021</v>
       </c>
       <c r="P576" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="577" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A577" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B577" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C577" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="C577" s="2" t="s">
+      <c r="D577" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D577" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="E577" s="2" t="s">
         <v>19</v>
       </c>
@@ -29619,206 +29619,206 @@
         <v>2021</v>
       </c>
       <c r="P577" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="578" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A578" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C578" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="C578" s="2" t="s">
+      <c r="D578" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="D578" s="2" t="s">
+      <c r="E578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H578" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O578" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P578" s="3" t="s">
         <v>563</v>
-      </c>
-      <c r="E578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H578" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O578" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P578" s="3" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="579" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A579" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C579" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="C579" s="2" t="s">
+      <c r="D579" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="D579" s="2" t="s">
+      <c r="E579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G579" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O579" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P579" s="3" t="s">
         <v>567</v>
-      </c>
-      <c r="E579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G579" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O579" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P579" s="3" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="580" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A580" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D580" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K580" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O580" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P580" s="3" t="s">
         <v>567</v>
-      </c>
-      <c r="E580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K580" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O580" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P580" s="3" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="581" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A581" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C581" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D581" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L581" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O581" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P581" s="3" t="s">
         <v>567</v>
-      </c>
-      <c r="E581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L581" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O581" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P581" s="3" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="582" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A582" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C582" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C582" s="2" t="s">
+      <c r="D582" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="D582" s="2" t="s">
-        <v>572</v>
       </c>
       <c r="E582" s="2" t="s">
         <v>18</v>
@@ -29854,18 +29854,18 @@
         <v>2020</v>
       </c>
       <c r="P582" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="583" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A583" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C583" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="C583" s="2" t="s">
+      <c r="D583" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="D583" s="2" t="s">
-        <v>572</v>
       </c>
       <c r="E583" s="2" t="s">
         <v>19</v>
@@ -29901,18 +29901,18 @@
         <v>2020</v>
       </c>
       <c r="P583" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="584" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A584" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C584" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D584" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E584" s="2" t="s">
         <v>19</v>
@@ -29948,1005 +29948,1005 @@
         <v>2020</v>
       </c>
       <c r="P584" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="585" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A585" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C585" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D585" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="E585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L585" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O585" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P585" s="3" t="s">
         <v>572</v>
-      </c>
-      <c r="E585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L585" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O585" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P585" s="3" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="586" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A586" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C586" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="C586" s="2" t="s">
+      <c r="D586" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="D586" s="2" t="s">
+      <c r="E586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J586" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O586" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P586" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J586" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O586" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P586" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="587" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A587" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="C587" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="C587" s="2" t="s">
+      <c r="D587" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="D587" s="2" t="s">
+      <c r="E587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I587" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O587" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P587" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I587" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O587" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P587" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="588" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A588" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C588" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D588" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K588" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O588" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P588" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K588" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O588" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P588" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="589" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A589" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C589" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D589" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L589" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O589" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P589" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L589" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O589" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P589" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="590" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A590" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C590" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D590" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N590" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O590" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P590" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N590" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O590" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P590" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="591" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A591" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C591" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D591" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L591" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O591" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P591" s="3" t="s">
         <v>578</v>
-      </c>
-      <c r="E591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L591" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O591" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P591" s="3" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="592" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A592" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="C592" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C592" s="2" t="s">
+      <c r="D592" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="D592" s="2" t="s">
+      <c r="E592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L592" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O592" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P592" s="3" t="s">
         <v>584</v>
-      </c>
-      <c r="E592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L592" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O592" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P592" s="3" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="593" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A593" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C593" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C593" s="2" t="s">
+      <c r="D593" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E593" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O593" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P593" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="D593" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="E593" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O593" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P593" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="594" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A594" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C594" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C594" s="2" t="s">
+      <c r="D594" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G594" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O594" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P594" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="D594" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="E594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G594" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O594" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P594" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="595" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A595" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C595" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C595" s="2" t="s">
+      <c r="D595" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L595" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O595" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P595" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="D595" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="E595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L595" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O595" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P595" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="596" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A596" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C596" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C596" s="2" t="s">
+      <c r="D596" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M596" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O596" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P596" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="D596" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="E596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M596" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O596" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P596" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="597" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A597" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C597" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C597" s="2" t="s">
+      <c r="D597" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N597" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O597" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P597" s="3" t="s">
         <v>587</v>
-      </c>
-      <c r="D597" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="E597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N597" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O597" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P597" s="3" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="598" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A598" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C598" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C598" s="2" t="s">
+      <c r="D598" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D598" s="2" t="s">
+      <c r="E598" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O598" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P598" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E598" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O598" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P598" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="599" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A599" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C599" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C599" s="2" t="s">
+      <c r="D599" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D599" s="2" t="s">
+      <c r="E599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G599" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O599" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P599" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G599" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O599" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P599" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="600" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A600" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C600" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C600" s="2" t="s">
+      <c r="D600" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D600" s="2" t="s">
+      <c r="E600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F600" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O600" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P600" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F600" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O600" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P600" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="601" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A601" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C601" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C601" s="2" t="s">
+      <c r="D601" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D601" s="2" t="s">
+      <c r="E601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K601" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O601" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P601" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K601" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O601" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P601" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="602" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A602" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C602" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C602" s="2" t="s">
+      <c r="D602" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D602" s="2" t="s">
+      <c r="E602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L602" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O602" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P602" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L602" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O602" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P602" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="603" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A603" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C603" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C603" s="2" t="s">
+      <c r="D603" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D603" s="2" t="s">
+      <c r="E603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M603" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O603" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P603" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M603" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O603" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P603" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="604" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A604" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C604" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="C604" s="2" t="s">
+      <c r="D604" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D604" s="2" t="s">
+      <c r="E604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N604" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O604" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P604" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="E604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N604" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O604" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P604" s="3" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="605" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A605" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C605" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C605" s="2" t="s">
+      <c r="D605" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D605" s="2" t="s">
+      <c r="E605" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O605" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P605" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="E605" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O605" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P605" s="3" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="606" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A606" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C606" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C606" s="2" t="s">
+      <c r="D606" s="2" t="s">
         <v>594</v>
-      </c>
-      <c r="D606" s="2" t="s">
-        <v>595</v>
       </c>
       <c r="E606" s="2" t="s">
         <v>19</v>
@@ -30982,101 +30982,101 @@
         <v>2020</v>
       </c>
       <c r="P606" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="607" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A607" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C607" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C607" s="2" t="s">
+      <c r="D607" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D607" s="2" t="s">
+      <c r="E607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K607" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O607" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P607" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="E607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K607" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O607" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P607" s="3" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="608" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A608" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C608" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="C608" s="2" t="s">
+      <c r="D608" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D608" s="2" t="s">
+      <c r="E608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L608" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O608" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P608" s="3" t="s">
         <v>595</v>
-      </c>
-      <c r="E608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L608" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O608" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P608" s="3" t="s">
-        <v>596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update url for Wakefield College
</commit_message>
<xml_diff>
--- a/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
+++ b/sfa.Tl.Marketing.Communication.DataLoad/Provider Data/Full Provider Data 2020 - 2021 (campaign site).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esfa\tl-marketing-and-communication\sfa.Tl.Marketing.Communication.DataLoad\Provider Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3BD05E-4008-40A2-AEF2-515455E3898B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDB702C-40AE-4A54-B123-79E1CBF5CDB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31725" yWindow="2505" windowWidth="19350" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40365" yWindow="5580" windowWidth="23685" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Provider Data 2020 - 2021" sheetId="1" r:id="rId1"/>
@@ -1651,9 +1651,6 @@
     <t>Wakefield</t>
   </si>
   <si>
-    <t>https://courses.wakefield.ac.uk/</t>
-  </si>
-  <si>
     <t>Walsall College</t>
   </si>
   <si>
@@ -1820,6 +1817,9 @@
   </si>
   <si>
     <t>https://www.ucb.ac.uk/study/college/introducing-new-t-levels/</t>
+  </si>
+  <si>
+    <t>https://www.wakefield.ac.uk/study-with-us/school-leavers/t-levels</t>
   </si>
 </sst>
 </file>
@@ -2205,9 +2205,9 @@
   </sheetPr>
   <dimension ref="A1:P608"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G557" sqref="A557:XFD557"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A556" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P560" sqref="P560:P562"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2240,7 +2240,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -21246,7 +21246,7 @@
         <v>2020</v>
       </c>
       <c r="P400" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="401" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -21293,7 +21293,7 @@
         <v>2021</v>
       </c>
       <c r="P401" s="4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="402" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22280,7 +22280,7 @@
         <v>2021</v>
       </c>
       <c r="P422" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="423" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22327,7 +22327,7 @@
         <v>2021</v>
       </c>
       <c r="P423" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="424" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -22374,7 +22374,7 @@
         <v>2020</v>
       </c>
       <c r="P424" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="425" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28667,7 +28667,7 @@
         <v>2021</v>
       </c>
       <c r="P557" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="558" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28714,7 +28714,7 @@
         <v>2021</v>
       </c>
       <c r="P558" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="559" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28807,8 +28807,8 @@
       <c r="O560" s="2">
         <v>2021</v>
       </c>
-      <c r="P560" s="3" t="s">
-        <v>543</v>
+      <c r="P560" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="561" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28854,8 +28854,8 @@
       <c r="O561" s="2">
         <v>2021</v>
       </c>
-      <c r="P561" s="3" t="s">
-        <v>543</v>
+      <c r="P561" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="562" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
@@ -28901,19 +28901,19 @@
       <c r="O562" s="2">
         <v>2021</v>
       </c>
-      <c r="P562" s="3" t="s">
-        <v>543</v>
+      <c r="P562" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="563" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A563" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C563" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C563" s="2" t="s">
+      <c r="D563" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="D563" s="2" t="s">
-        <v>546</v>
       </c>
       <c r="E563" s="2" t="s">
         <v>18</v>
@@ -28949,112 +28949,112 @@
         <v>2020</v>
       </c>
       <c r="P563" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="564" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A564" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C564" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C564" s="2" t="s">
+      <c r="D564" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D564" s="2" t="s">
+      <c r="E564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G564" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N564" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O564" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P564" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G564" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N564" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O564" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P564" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="565" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A565" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C565" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C565" s="2" t="s">
+      <c r="D565" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D565" s="2" t="s">
+      <c r="E565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F565" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N565" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O565" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P565" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F565" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N565" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O565" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P565" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="566" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A566" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C566" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C566" s="2" t="s">
+      <c r="D566" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="D566" s="2" t="s">
-        <v>546</v>
       </c>
       <c r="E566" s="2" t="s">
         <v>19</v>
@@ -29090,159 +29090,159 @@
         <v>2020</v>
       </c>
       <c r="P566" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="567" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A567" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C567" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C567" s="2" t="s">
+      <c r="D567" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D567" s="2" t="s">
+      <c r="E567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L567" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N567" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O567" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P567" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L567" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N567" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O567" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P567" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="568" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A568" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C568" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C568" s="2" t="s">
+      <c r="D568" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D568" s="2" t="s">
+      <c r="E568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M568" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N568" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O568" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P568" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M568" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N568" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O568" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P568" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="569" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A569" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C569" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C569" s="2" t="s">
+      <c r="D569" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D569" s="2" t="s">
+      <c r="E569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M569" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N569" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O569" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P569" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M569" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N569" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O569" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P569" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="570" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A570" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C570" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D570" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E570" s="2" t="s">
         <v>19</v>
@@ -29278,213 +29278,213 @@
         <v>2020</v>
       </c>
       <c r="P570" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="571" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A571" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C571" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D571" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I571" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N571" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O571" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P571" s="3" t="s">
         <v>546</v>
-      </c>
-      <c r="E571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I571" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N571" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O571" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P571" s="3" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="572" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A572" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C572" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="C572" s="2" t="s">
+      <c r="D572" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F572" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N572" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O572" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P572" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="D572" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="E572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F572" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N572" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O572" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P572" s="3" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="573" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A573" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C573" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="C573" s="2" t="s">
+      <c r="D573" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E573" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N573" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O573" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P573" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="D573" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="E573" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N573" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O573" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P573" s="3" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="574" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A574" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B574" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B574" s="2" t="s">
+      <c r="C574" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="C574" s="2" t="s">
+      <c r="D574" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="D574" s="2" t="s">
+      <c r="E574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G574" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N574" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O574" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P574" s="3" t="s">
         <v>555</v>
-      </c>
-      <c r="E574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G574" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N574" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O574" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P574" s="3" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="575" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A575" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B575" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C575" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C575" s="2" t="s">
+      <c r="D575" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D575" s="2" t="s">
-        <v>559</v>
-      </c>
       <c r="E575" s="2" t="s">
         <v>19</v>
       </c>
@@ -29519,22 +29519,22 @@
         <v>2021</v>
       </c>
       <c r="P575" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="576" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A576" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B576" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C576" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C576" s="2" t="s">
+      <c r="D576" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D576" s="2" t="s">
-        <v>559</v>
-      </c>
       <c r="E576" s="2" t="s">
         <v>18</v>
       </c>
@@ -29569,22 +29569,22 @@
         <v>2021</v>
       </c>
       <c r="P576" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="577" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A577" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B577" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C577" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C577" s="2" t="s">
+      <c r="D577" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D577" s="2" t="s">
-        <v>559</v>
-      </c>
       <c r="E577" s="2" t="s">
         <v>19</v>
       </c>
@@ -29619,206 +29619,206 @@
         <v>2021</v>
       </c>
       <c r="P577" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="578" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A578" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C578" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="C578" s="2" t="s">
+      <c r="D578" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="D578" s="2" t="s">
+      <c r="E578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H578" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N578" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O578" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P578" s="3" t="s">
         <v>562</v>
-      </c>
-      <c r="E578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H578" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N578" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O578" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P578" s="3" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="579" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A579" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C579" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="C579" s="2" t="s">
+      <c r="D579" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="D579" s="2" t="s">
+      <c r="E579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G579" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N579" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O579" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P579" s="3" t="s">
         <v>566</v>
-      </c>
-      <c r="E579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G579" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N579" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O579" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P579" s="3" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="580" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A580" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D580" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K580" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N580" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O580" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P580" s="3" t="s">
         <v>566</v>
-      </c>
-      <c r="E580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K580" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N580" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O580" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P580" s="3" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="581" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A581" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C581" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D581" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L581" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N581" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O581" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P581" s="3" t="s">
         <v>566</v>
-      </c>
-      <c r="E581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L581" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N581" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O581" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P581" s="3" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="582" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A582" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C582" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="C582" s="2" t="s">
+      <c r="D582" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="D582" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="E582" s="2" t="s">
         <v>18</v>
@@ -29854,18 +29854,18 @@
         <v>2020</v>
       </c>
       <c r="P582" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="583" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A583" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C583" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="C583" s="2" t="s">
+      <c r="D583" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="D583" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="E583" s="2" t="s">
         <v>19</v>
@@ -29901,18 +29901,18 @@
         <v>2020</v>
       </c>
       <c r="P583" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="584" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A584" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C584" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D584" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E584" s="2" t="s">
         <v>19</v>
@@ -29948,1005 +29948,1005 @@
         <v>2020</v>
       </c>
       <c r="P584" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="585" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A585" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C585" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D585" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="E585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L585" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N585" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O585" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P585" s="3" t="s">
         <v>571</v>
-      </c>
-      <c r="E585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L585" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N585" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O585" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P585" s="3" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="586" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A586" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C586" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="C586" s="2" t="s">
+      <c r="D586" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="D586" s="2" t="s">
+      <c r="E586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J586" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N586" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O586" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P586" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J586" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N586" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O586" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P586" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="587" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A587" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C587" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="C587" s="2" t="s">
+      <c r="D587" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="D587" s="2" t="s">
+      <c r="E587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I587" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N587" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O587" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P587" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I587" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N587" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O587" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P587" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="588" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A588" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C588" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D588" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K588" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N588" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O588" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P588" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K588" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N588" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O588" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P588" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="589" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A589" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C589" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D589" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L589" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N589" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O589" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P589" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L589" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N589" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O589" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P589" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="590" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A590" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C590" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D590" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M590" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N590" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O590" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P590" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M590" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N590" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O590" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P590" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="591" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A591" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C591" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D591" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="E591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L591" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N591" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O591" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P591" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="E591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L591" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N591" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O591" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P591" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="592" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A592" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="C592" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="C592" s="2" t="s">
+      <c r="D592" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="D592" s="2" t="s">
+      <c r="E592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L592" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N592" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O592" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P592" s="3" t="s">
         <v>583</v>
-      </c>
-      <c r="E592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L592" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N592" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O592" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P592" s="3" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="593" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A593" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C593" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C593" s="2" t="s">
+      <c r="D593" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E593" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N593" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O593" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P593" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="D593" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="E593" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N593" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O593" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P593" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="594" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A594" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C594" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C594" s="2" t="s">
+      <c r="D594" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G594" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N594" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O594" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P594" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="D594" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="E594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G594" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N594" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O594" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P594" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="595" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A595" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C595" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C595" s="2" t="s">
+      <c r="D595" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L595" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N595" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O595" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P595" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="D595" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="E595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L595" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N595" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O595" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P595" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="596" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A596" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C596" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C596" s="2" t="s">
+      <c r="D596" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M596" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N596" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O596" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P596" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="D596" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="E596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M596" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N596" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O596" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P596" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="597" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A597" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C597" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C597" s="2" t="s">
+      <c r="D597" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M597" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N597" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O597" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P597" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="D597" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="E597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M597" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N597" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O597" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P597" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="598" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A598" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C598" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C598" s="2" t="s">
+      <c r="D598" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D598" s="2" t="s">
+      <c r="E598" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N598" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O598" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P598" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E598" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N598" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O598" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P598" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="599" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A599" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C599" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C599" s="2" t="s">
+      <c r="D599" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D599" s="2" t="s">
+      <c r="E599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G599" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N599" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O599" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P599" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G599" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N599" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O599" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P599" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="600" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A600" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C600" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C600" s="2" t="s">
+      <c r="D600" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D600" s="2" t="s">
+      <c r="E600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F600" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N600" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O600" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P600" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F600" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N600" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O600" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P600" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="601" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A601" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C601" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C601" s="2" t="s">
+      <c r="D601" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D601" s="2" t="s">
+      <c r="E601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K601" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N601" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O601" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P601" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K601" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N601" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O601" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P601" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="602" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A602" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C602" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C602" s="2" t="s">
+      <c r="D602" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D602" s="2" t="s">
+      <c r="E602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L602" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N602" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O602" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P602" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L602" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N602" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O602" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P602" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="603" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A603" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C603" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C603" s="2" t="s">
+      <c r="D603" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D603" s="2" t="s">
+      <c r="E603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M603" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N603" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O603" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P603" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M603" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N603" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O603" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P603" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="604" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A604" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C604" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="C604" s="2" t="s">
+      <c r="D604" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D604" s="2" t="s">
+      <c r="E604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M604" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N604" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O604" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P604" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="E604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M604" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N604" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O604" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P604" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="605" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A605" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C605" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C605" s="2" t="s">
+      <c r="D605" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D605" s="2" t="s">
+      <c r="E605" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N605" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O605" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P605" s="3" t="s">
         <v>594</v>
-      </c>
-      <c r="E605" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N605" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O605" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P605" s="3" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="606" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A606" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C606" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C606" s="2" t="s">
+      <c r="D606" s="2" t="s">
         <v>593</v>
-      </c>
-      <c r="D606" s="2" t="s">
-        <v>594</v>
       </c>
       <c r="E606" s="2" t="s">
         <v>19</v>
@@ -30982,101 +30982,101 @@
         <v>2020</v>
       </c>
       <c r="P606" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="607" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A607" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C607" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C607" s="2" t="s">
+      <c r="D607" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D607" s="2" t="s">
+      <c r="E607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K607" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N607" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O607" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P607" s="3" t="s">
         <v>594</v>
-      </c>
-      <c r="E607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K607" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N607" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O607" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P607" s="3" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="608" spans="1:16" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A608" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C608" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C608" s="2" t="s">
+      <c r="D608" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D608" s="2" t="s">
+      <c r="E608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L608" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N608" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O608" s="2">
+        <v>2021</v>
+      </c>
+      <c r="P608" s="3" t="s">
         <v>594</v>
-      </c>
-      <c r="E608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L608" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N608" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O608" s="2">
-        <v>2021</v>
-      </c>
-      <c r="P608" s="3" t="s">
-        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -31634,60 +31634,59 @@
     <hyperlink ref="P558" r:id="rId551" xr:uid="{00000000-0004-0000-0000-00002B020000}"/>
     <hyperlink ref="P559" r:id="rId552" xr:uid="{00000000-0004-0000-0000-00002C020000}"/>
     <hyperlink ref="P560" r:id="rId553" xr:uid="{00000000-0004-0000-0000-00002D020000}"/>
-    <hyperlink ref="P561" r:id="rId554" xr:uid="{00000000-0004-0000-0000-00002E020000}"/>
-    <hyperlink ref="P562" r:id="rId555" xr:uid="{00000000-0004-0000-0000-00002F020000}"/>
-    <hyperlink ref="P563" r:id="rId556" xr:uid="{00000000-0004-0000-0000-000030020000}"/>
-    <hyperlink ref="P564" r:id="rId557" xr:uid="{00000000-0004-0000-0000-000031020000}"/>
-    <hyperlink ref="P565" r:id="rId558" xr:uid="{00000000-0004-0000-0000-000032020000}"/>
-    <hyperlink ref="P566" r:id="rId559" xr:uid="{00000000-0004-0000-0000-000033020000}"/>
-    <hyperlink ref="P567" r:id="rId560" xr:uid="{00000000-0004-0000-0000-000034020000}"/>
-    <hyperlink ref="P568" r:id="rId561" xr:uid="{00000000-0004-0000-0000-000035020000}"/>
-    <hyperlink ref="P569" r:id="rId562" xr:uid="{00000000-0004-0000-0000-000036020000}"/>
-    <hyperlink ref="P570" r:id="rId563" xr:uid="{00000000-0004-0000-0000-000037020000}"/>
-    <hyperlink ref="P571" r:id="rId564" xr:uid="{00000000-0004-0000-0000-000038020000}"/>
-    <hyperlink ref="P572" r:id="rId565" xr:uid="{00000000-0004-0000-0000-000039020000}"/>
-    <hyperlink ref="P573" r:id="rId566" xr:uid="{00000000-0004-0000-0000-00003A020000}"/>
-    <hyperlink ref="P574" r:id="rId567" xr:uid="{00000000-0004-0000-0000-00003B020000}"/>
-    <hyperlink ref="P575" r:id="rId568" xr:uid="{00000000-0004-0000-0000-00003C020000}"/>
-    <hyperlink ref="P576" r:id="rId569" xr:uid="{00000000-0004-0000-0000-00003D020000}"/>
-    <hyperlink ref="P577" r:id="rId570" xr:uid="{00000000-0004-0000-0000-00003E020000}"/>
-    <hyperlink ref="P578" r:id="rId571" xr:uid="{00000000-0004-0000-0000-00003F020000}"/>
-    <hyperlink ref="P579" r:id="rId572" xr:uid="{00000000-0004-0000-0000-000040020000}"/>
-    <hyperlink ref="P580" r:id="rId573" xr:uid="{00000000-0004-0000-0000-000041020000}"/>
-    <hyperlink ref="P581" r:id="rId574" xr:uid="{00000000-0004-0000-0000-000042020000}"/>
-    <hyperlink ref="P582" r:id="rId575" xr:uid="{00000000-0004-0000-0000-000043020000}"/>
-    <hyperlink ref="P583" r:id="rId576" xr:uid="{00000000-0004-0000-0000-000044020000}"/>
-    <hyperlink ref="P584" r:id="rId577" xr:uid="{00000000-0004-0000-0000-000045020000}"/>
-    <hyperlink ref="P585" r:id="rId578" xr:uid="{00000000-0004-0000-0000-000046020000}"/>
-    <hyperlink ref="P586" r:id="rId579" xr:uid="{00000000-0004-0000-0000-000047020000}"/>
-    <hyperlink ref="P587" r:id="rId580" xr:uid="{00000000-0004-0000-0000-000048020000}"/>
-    <hyperlink ref="P588" r:id="rId581" xr:uid="{00000000-0004-0000-0000-000049020000}"/>
-    <hyperlink ref="P589" r:id="rId582" xr:uid="{00000000-0004-0000-0000-00004A020000}"/>
-    <hyperlink ref="P590" r:id="rId583" xr:uid="{00000000-0004-0000-0000-00004B020000}"/>
-    <hyperlink ref="P591" r:id="rId584" xr:uid="{00000000-0004-0000-0000-00004C020000}"/>
-    <hyperlink ref="P592" r:id="rId585" xr:uid="{00000000-0004-0000-0000-00004D020000}"/>
-    <hyperlink ref="P593" r:id="rId586" xr:uid="{00000000-0004-0000-0000-00004E020000}"/>
-    <hyperlink ref="P594" r:id="rId587" xr:uid="{00000000-0004-0000-0000-00004F020000}"/>
-    <hyperlink ref="P595" r:id="rId588" xr:uid="{00000000-0004-0000-0000-000050020000}"/>
-    <hyperlink ref="P596" r:id="rId589" xr:uid="{00000000-0004-0000-0000-000051020000}"/>
-    <hyperlink ref="P597" r:id="rId590" xr:uid="{00000000-0004-0000-0000-000052020000}"/>
-    <hyperlink ref="P598" r:id="rId591" xr:uid="{00000000-0004-0000-0000-000053020000}"/>
-    <hyperlink ref="P599" r:id="rId592" xr:uid="{00000000-0004-0000-0000-000054020000}"/>
-    <hyperlink ref="P600" r:id="rId593" xr:uid="{00000000-0004-0000-0000-000055020000}"/>
-    <hyperlink ref="P601" r:id="rId594" xr:uid="{00000000-0004-0000-0000-000056020000}"/>
-    <hyperlink ref="P602" r:id="rId595" xr:uid="{00000000-0004-0000-0000-000057020000}"/>
-    <hyperlink ref="P603" r:id="rId596" xr:uid="{00000000-0004-0000-0000-000058020000}"/>
-    <hyperlink ref="P604" r:id="rId597" xr:uid="{00000000-0004-0000-0000-000059020000}"/>
-    <hyperlink ref="P605" r:id="rId598" xr:uid="{00000000-0004-0000-0000-00005A020000}"/>
-    <hyperlink ref="P606" r:id="rId599" xr:uid="{00000000-0004-0000-0000-00005B020000}"/>
-    <hyperlink ref="P607" r:id="rId600" xr:uid="{00000000-0004-0000-0000-00005C020000}"/>
-    <hyperlink ref="P608" r:id="rId601" xr:uid="{00000000-0004-0000-0000-00005D020000}"/>
-    <hyperlink ref="P148" r:id="rId602" xr:uid="{32E39374-F929-402C-9450-D1267E2F204C}"/>
-    <hyperlink ref="P399" r:id="rId603" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="P400" r:id="rId604" xr:uid="{2AB82485-73BC-4FA4-80C9-24FDE180DE05}"/>
-    <hyperlink ref="P422:P424" r:id="rId605" display="https://www.osfc.ac.uk/courses/digital-t-level/" xr:uid="{5F95BC6B-E320-42B3-9AAA-E18B5D75E9BE}"/>
+    <hyperlink ref="P563" r:id="rId554" xr:uid="{00000000-0004-0000-0000-000030020000}"/>
+    <hyperlink ref="P564" r:id="rId555" xr:uid="{00000000-0004-0000-0000-000031020000}"/>
+    <hyperlink ref="P565" r:id="rId556" xr:uid="{00000000-0004-0000-0000-000032020000}"/>
+    <hyperlink ref="P566" r:id="rId557" xr:uid="{00000000-0004-0000-0000-000033020000}"/>
+    <hyperlink ref="P567" r:id="rId558" xr:uid="{00000000-0004-0000-0000-000034020000}"/>
+    <hyperlink ref="P568" r:id="rId559" xr:uid="{00000000-0004-0000-0000-000035020000}"/>
+    <hyperlink ref="P569" r:id="rId560" xr:uid="{00000000-0004-0000-0000-000036020000}"/>
+    <hyperlink ref="P570" r:id="rId561" xr:uid="{00000000-0004-0000-0000-000037020000}"/>
+    <hyperlink ref="P571" r:id="rId562" xr:uid="{00000000-0004-0000-0000-000038020000}"/>
+    <hyperlink ref="P572" r:id="rId563" xr:uid="{00000000-0004-0000-0000-000039020000}"/>
+    <hyperlink ref="P573" r:id="rId564" xr:uid="{00000000-0004-0000-0000-00003A020000}"/>
+    <hyperlink ref="P574" r:id="rId565" xr:uid="{00000000-0004-0000-0000-00003B020000}"/>
+    <hyperlink ref="P575" r:id="rId566" xr:uid="{00000000-0004-0000-0000-00003C020000}"/>
+    <hyperlink ref="P576" r:id="rId567" xr:uid="{00000000-0004-0000-0000-00003D020000}"/>
+    <hyperlink ref="P577" r:id="rId568" xr:uid="{00000000-0004-0000-0000-00003E020000}"/>
+    <hyperlink ref="P578" r:id="rId569" xr:uid="{00000000-0004-0000-0000-00003F020000}"/>
+    <hyperlink ref="P579" r:id="rId570" xr:uid="{00000000-0004-0000-0000-000040020000}"/>
+    <hyperlink ref="P580" r:id="rId571" xr:uid="{00000000-0004-0000-0000-000041020000}"/>
+    <hyperlink ref="P581" r:id="rId572" xr:uid="{00000000-0004-0000-0000-000042020000}"/>
+    <hyperlink ref="P582" r:id="rId573" xr:uid="{00000000-0004-0000-0000-000043020000}"/>
+    <hyperlink ref="P583" r:id="rId574" xr:uid="{00000000-0004-0000-0000-000044020000}"/>
+    <hyperlink ref="P584" r:id="rId575" xr:uid="{00000000-0004-0000-0000-000045020000}"/>
+    <hyperlink ref="P585" r:id="rId576" xr:uid="{00000000-0004-0000-0000-000046020000}"/>
+    <hyperlink ref="P586" r:id="rId577" xr:uid="{00000000-0004-0000-0000-000047020000}"/>
+    <hyperlink ref="P587" r:id="rId578" xr:uid="{00000000-0004-0000-0000-000048020000}"/>
+    <hyperlink ref="P588" r:id="rId579" xr:uid="{00000000-0004-0000-0000-000049020000}"/>
+    <hyperlink ref="P589" r:id="rId580" xr:uid="{00000000-0004-0000-0000-00004A020000}"/>
+    <hyperlink ref="P590" r:id="rId581" xr:uid="{00000000-0004-0000-0000-00004B020000}"/>
+    <hyperlink ref="P591" r:id="rId582" xr:uid="{00000000-0004-0000-0000-00004C020000}"/>
+    <hyperlink ref="P592" r:id="rId583" xr:uid="{00000000-0004-0000-0000-00004D020000}"/>
+    <hyperlink ref="P593" r:id="rId584" xr:uid="{00000000-0004-0000-0000-00004E020000}"/>
+    <hyperlink ref="P594" r:id="rId585" xr:uid="{00000000-0004-0000-0000-00004F020000}"/>
+    <hyperlink ref="P595" r:id="rId586" xr:uid="{00000000-0004-0000-0000-000050020000}"/>
+    <hyperlink ref="P596" r:id="rId587" xr:uid="{00000000-0004-0000-0000-000051020000}"/>
+    <hyperlink ref="P597" r:id="rId588" xr:uid="{00000000-0004-0000-0000-000052020000}"/>
+    <hyperlink ref="P598" r:id="rId589" xr:uid="{00000000-0004-0000-0000-000053020000}"/>
+    <hyperlink ref="P599" r:id="rId590" xr:uid="{00000000-0004-0000-0000-000054020000}"/>
+    <hyperlink ref="P600" r:id="rId591" xr:uid="{00000000-0004-0000-0000-000055020000}"/>
+    <hyperlink ref="P601" r:id="rId592" xr:uid="{00000000-0004-0000-0000-000056020000}"/>
+    <hyperlink ref="P602" r:id="rId593" xr:uid="{00000000-0004-0000-0000-000057020000}"/>
+    <hyperlink ref="P603" r:id="rId594" xr:uid="{00000000-0004-0000-0000-000058020000}"/>
+    <hyperlink ref="P604" r:id="rId595" xr:uid="{00000000-0004-0000-0000-000059020000}"/>
+    <hyperlink ref="P605" r:id="rId596" xr:uid="{00000000-0004-0000-0000-00005A020000}"/>
+    <hyperlink ref="P606" r:id="rId597" xr:uid="{00000000-0004-0000-0000-00005B020000}"/>
+    <hyperlink ref="P607" r:id="rId598" xr:uid="{00000000-0004-0000-0000-00005C020000}"/>
+    <hyperlink ref="P608" r:id="rId599" xr:uid="{00000000-0004-0000-0000-00005D020000}"/>
+    <hyperlink ref="P148" r:id="rId600" xr:uid="{32E39374-F929-402C-9450-D1267E2F204C}"/>
+    <hyperlink ref="P399" r:id="rId601" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="P400" r:id="rId602" xr:uid="{2AB82485-73BC-4FA4-80C9-24FDE180DE05}"/>
+    <hyperlink ref="P422:P424" r:id="rId603" display="https://www.osfc.ac.uk/courses/digital-t-level/" xr:uid="{5F95BC6B-E320-42B3-9AAA-E18B5D75E9BE}"/>
+    <hyperlink ref="P561:P562" r:id="rId604" display="https://www.wakefield.ac.uk/study-with-us/school-leavers/t-levels" xr:uid="{DC28D138-C018-4C84-81C2-1ED512EA2C1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId606"/>
+  <pageSetup orientation="portrait" r:id="rId605"/>
 </worksheet>
 </file>
</xml_diff>